<commit_message>
summary table with all parameters and estimates
</commit_message>
<xml_diff>
--- a/writing/Manuscript_Tables.xlsx
+++ b/writing/Manuscript_Tables.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/genoasullaway/Documents/GitHub/AYK_prey/writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDCF07FD-C4D7-F342-9019-F6FFA3A107CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE6C375A-1DF9-9344-B311-3951FB26D130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6960" yWindow="760" windowWidth="27600" windowHeight="19380" activeTab="1" xr2:uid="{15635B22-154F-5C4D-8D09-E55D0FC35932}"/>
+    <workbookView xWindow="14780" yWindow="760" windowWidth="19780" windowHeight="19380" xr2:uid="{15635B22-154F-5C4D-8D09-E55D0FC35932}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1 Priors" sheetId="4" r:id="rId1"/>
     <sheet name="Table 2 Covariates" sheetId="3" r:id="rId2"/>
     <sheet name="Supplement Table 1" sheetId="5" r:id="rId3"/>
-    <sheet name="OLD - ignore" sheetId="1" r:id="rId4"/>
+    <sheet name="Supplement Table 2 " sheetId="6" r:id="rId4"/>
+    <sheet name="OLD - ignore" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="127">
   <si>
     <t>Stage</t>
   </si>
@@ -436,6 +437,27 @@
   </si>
   <si>
     <t>Annual index, 2002-2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parameter </t>
+  </si>
+  <si>
+    <t>Parameter Description</t>
+  </si>
+  <si>
+    <t>Parameter Mean Estimate</t>
+  </si>
+  <si>
+    <t>95% CI</t>
+  </si>
+  <si>
+    <t>R Hat</t>
+  </si>
+  <si>
+    <t>Effective Sample Size</t>
+  </si>
+  <si>
+    <t>currently fixed:</t>
   </si>
 </sst>
 </file>
@@ -2112,7 +2134,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>17956</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>11385</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="100156" cy="173766"/>
@@ -2242,7 +2264,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>9200</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>2628</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="141256" cy="173766"/>
@@ -2558,7 +2580,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>22334</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>28904</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="172035" cy="173702"/>
@@ -2712,352 +2734,8 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>44231</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>7006</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="284886" cy="182871"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="14" name="TextBox 13">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EDD8896-0B5A-9870-9DA3-179FFD601EA8}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="871921" y="1417144"/>
-              <a:ext cx="284886" cy="182871"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a14:m>
-                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:oMathParaPr>
-                    <m:jc m:val="centerGroup"/>
-                  </m:oMathParaPr>
-                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                    <m:sSub>
-                      <m:sSubPr>
-                        <m:ctrlPr>
-                          <a:rPr lang="en-US" sz="1100" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                        </m:ctrlPr>
-                      </m:sSubPr>
-                      <m:e>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝜂</m:t>
-                        </m:r>
-                      </m:e>
-                      <m:sub>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑠</m:t>
-                        </m:r>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>=</m:t>
-                        </m:r>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑗</m:t>
-                        </m:r>
-                      </m:sub>
-                    </m:sSub>
-                  </m:oMath>
-                </m:oMathPara>
-              </a14:m>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="14" name="TextBox 13">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EDD8896-0B5A-9870-9DA3-179FFD601EA8}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="871921" y="1417144"/>
-              <a:ext cx="284886" cy="182871"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>𝜂_(</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>𝑠=𝑗)</a:t>
-              </a:r>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>25838</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>198820</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="331053" cy="173702"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="15" name="TextBox 14">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87B5AF8D-A9A9-ED4E-BFBB-EA896709B184}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="853528" y="1608958"/>
-              <a:ext cx="331053" cy="173702"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a14:m>
-                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:oMathParaPr>
-                    <m:jc m:val="centerGroup"/>
-                  </m:oMathParaPr>
-                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                    <m:sSub>
-                      <m:sSubPr>
-                        <m:ctrlPr>
-                          <a:rPr lang="en-US" sz="1100" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                        </m:ctrlPr>
-                      </m:sSubPr>
-                      <m:e>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝜂</m:t>
-                        </m:r>
-                      </m:e>
-                      <m:sub>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑠</m:t>
-                        </m:r>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>=</m:t>
-                        </m:r>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑚</m:t>
-                        </m:r>
-                      </m:sub>
-                    </m:sSub>
-                  </m:oMath>
-                </m:oMathPara>
-              </a14:m>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="15" name="TextBox 14">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87B5AF8D-A9A9-ED4E-BFBB-EA896709B184}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="853528" y="1608958"/>
-              <a:ext cx="331053" cy="173702"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>𝜂_(</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>𝑠=𝑚)</a:t>
-              </a:r>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
       <xdr:colOff>31823</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>2626</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="106632" cy="173702"/>
@@ -3185,7 +2863,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>31823</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>8829</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="182614" cy="173702"/>
@@ -3340,7 +3018,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>43794</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>17224</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="128112" cy="173702"/>
@@ -3455,6 +3133,352 @@
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
                 <a:t>𝐷</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>44231</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>7006</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="284886" cy="182871"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BEB458A6-E310-2A4A-B504-A464DB3641CB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="866428" y="1717468"/>
+              <a:ext cx="284886" cy="182871"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝜂</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑠</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>=</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑗</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BEB458A6-E310-2A4A-B504-A464DB3641CB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="866428" y="1717468"/>
+              <a:ext cx="284886" cy="182871"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝜂_(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑠=𝑗)</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>25838</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>198820</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="331053" cy="173702"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10" name="TextBox 9">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E07D85B6-F39C-0348-AC5C-801AB8E792F4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="848035" y="1909282"/>
+              <a:ext cx="331053" cy="173702"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝜂</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑠</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>=</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑚</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10" name="TextBox 9">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E07D85B6-F39C-0348-AC5C-801AB8E792F4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="848035" y="1909282"/>
+              <a:ext cx="331053" cy="173702"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝜂_(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑠=𝑚)</a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="1100"/>
             </a:p>
@@ -3784,10 +3808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F6D1E8C-B800-DB41-95B4-3695A974BBA7}">
-  <dimension ref="B1:D19"/>
+  <dimension ref="B1:D24"/>
   <sheetViews>
-    <sheetView zoomScale="173" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" zoomScale="173" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3867,83 +3891,88 @@
     <row r="8" spans="2:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="67"/>
       <c r="C8" s="60" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D8" s="68" t="s">
-        <v>107</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B9" s="67"/>
-      <c r="C9" s="60" t="s">
-        <v>82</v>
+      <c r="C9" s="61" t="s">
+        <v>85</v>
       </c>
       <c r="D9" s="68" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="17" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="34" x14ac:dyDescent="0.2">
       <c r="B10" s="67"/>
-      <c r="C10" s="60" t="s">
-        <v>83</v>
+      <c r="C10" s="61" t="s">
+        <v>84</v>
       </c>
       <c r="D10" s="68" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:4" ht="34" x14ac:dyDescent="0.2">
       <c r="B11" s="67"/>
       <c r="C11" s="61" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="D11" s="68" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" ht="34" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B12" s="67"/>
-      <c r="C12" s="61" t="s">
-        <v>84</v>
+      <c r="C12" s="58" t="s">
+        <v>110</v>
       </c>
       <c r="D12" s="68" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="B13" s="67"/>
-      <c r="C13" s="61" t="s">
-        <v>109</v>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="69"/>
+      <c r="C13" s="62" t="s">
+        <v>108</v>
       </c>
       <c r="D13" s="68" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B14" s="67"/>
-      <c r="C14" s="58" t="s">
-        <v>110</v>
-      </c>
-      <c r="D14" s="68" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="69"/>
-      <c r="C15" s="62" t="s">
-        <v>108</v>
-      </c>
-      <c r="D15" s="68" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="C18" s="63" t="s">
+    <row r="16" spans="2:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="C16" s="63" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="19" spans="3:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="C19" s="64" t="s">
+    <row r="17" spans="2:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="C17" s="64" t="s">
         <v>106</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B22" s="45" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B23" s="67"/>
+      <c r="C23" s="60" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" s="68" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B24" s="67"/>
+      <c r="C24" s="60" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" s="68" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -3956,7 +3985,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C922C39-C49D-8D4D-BCBE-7247337ED328}">
   <dimension ref="B1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="164" workbookViewId="0">
+    <sheetView topLeftCell="C7" zoomScale="164" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -4330,6 +4359,53 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1D8EA89-DADA-994F-B9EB-DFFAA747018D}">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" customWidth="1"/>
+    <col min="5" max="5" width="26" customWidth="1"/>
+    <col min="6" max="6" width="24.6640625" customWidth="1"/>
+    <col min="7" max="7" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{084D3D18-8C71-464C-A320-63E682CA5315}">
   <dimension ref="B1:I12"/>
   <sheetViews>

</xml_diff>

<commit_message>
This is a good run, estimate all sigmas
just to try bc currently would like them in the tables
some messing with priors to be done, but looks like a better run a bit...
</commit_message>
<xml_diff>
--- a/writing/Manuscript_Tables.xlsx
+++ b/writing/Manuscript_Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/genoasullaway/Documents/GitHub/AYK_prey/writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE6C375A-1DF9-9344-B311-3951FB26D130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC0EB2EA-2670-D549-B648-68A0B5D02811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14780" yWindow="760" windowWidth="19780" windowHeight="19380" xr2:uid="{15635B22-154F-5C4D-8D09-E55D0FC35932}"/>
+    <workbookView xWindow="14120" yWindow="760" windowWidth="20660" windowHeight="20080" activeTab="3" xr2:uid="{15635B22-154F-5C4D-8D09-E55D0FC35932}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1 Priors" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="128">
   <si>
     <t>Stage</t>
   </si>
@@ -310,9 +310,6 @@
     <t>Carrying capacity for marine stage</t>
   </si>
   <si>
-    <t>Selectivity</t>
-  </si>
-  <si>
     <t>Log-normal standard deviation for instantaneous fishing mortality</t>
   </si>
   <si>
@@ -439,9 +436,6 @@
     <t>Annual index, 2002-2022</t>
   </si>
   <si>
-    <t xml:space="preserve">Parameter </t>
-  </si>
-  <si>
     <t>Parameter Description</t>
   </si>
   <si>
@@ -458,6 +452,15 @@
   </si>
   <si>
     <t>currently fixed:</t>
+  </si>
+  <si>
+    <t>Log-normal age-specific fishing selectivity</t>
+  </si>
+  <si>
+    <t>Parameter Notation</t>
+  </si>
+  <si>
+    <t>Parameter Group</t>
   </si>
 </sst>
 </file>
@@ -3810,8 +3813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F6D1E8C-B800-DB41-95B4-3695A974BBA7}">
   <dimension ref="B1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="173" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView zoomScale="173" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3882,7 +3885,7 @@
     <row r="7" spans="2:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="67"/>
       <c r="C7" s="60" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D7" s="68" t="s">
         <v>80</v>
@@ -3891,7 +3894,7 @@
     <row r="8" spans="2:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="67"/>
       <c r="C8" s="60" t="s">
-        <v>83</v>
+        <v>125</v>
       </c>
       <c r="D8" s="68" t="s">
         <v>77</v>
@@ -3900,7 +3903,7 @@
     <row r="9" spans="2:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B9" s="67"/>
       <c r="C9" s="61" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D9" s="68" t="s">
         <v>77</v>
@@ -3909,7 +3912,7 @@
     <row r="10" spans="2:4" ht="34" x14ac:dyDescent="0.2">
       <c r="B10" s="67"/>
       <c r="C10" s="61" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D10" s="68" t="s">
         <v>77</v>
@@ -3918,16 +3921,16 @@
     <row r="11" spans="2:4" ht="34" x14ac:dyDescent="0.2">
       <c r="B11" s="67"/>
       <c r="C11" s="61" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D11" s="68" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B12" s="67"/>
       <c r="C12" s="58" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D12" s="68" t="s">
         <v>78</v>
@@ -3936,7 +3939,7 @@
     <row r="13" spans="2:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="69"/>
       <c r="C13" s="62" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D13" s="68" t="s">
         <v>78</v>
@@ -3944,17 +3947,17 @@
     </row>
     <row r="16" spans="2:4" ht="17" x14ac:dyDescent="0.2">
       <c r="C16" s="63" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="34" x14ac:dyDescent="0.2">
       <c r="C17" s="64" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" s="45" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="17" x14ac:dyDescent="0.2">
@@ -3963,7 +3966,7 @@
         <v>81</v>
       </c>
       <c r="D23" s="68" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="17" x14ac:dyDescent="0.2">
@@ -3972,7 +3975,7 @@
         <v>82</v>
       </c>
       <c r="D24" s="68" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -3985,7 +3988,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C922C39-C49D-8D4D-BCBE-7247337ED328}">
   <dimension ref="B1:I15"/>
   <sheetViews>
-    <sheetView topLeftCell="C7" zoomScale="164" workbookViewId="0">
+    <sheetView zoomScale="75" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -4005,7 +4008,7 @@
   <sheetData>
     <row r="1" spans="2:9" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C1" s="47" t="s">
         <v>46</v>
@@ -4014,7 +4017,7 @@
         <v>61</v>
       </c>
       <c r="E1" s="47" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F1" s="47" t="s">
         <v>4</v>
@@ -4037,7 +4040,7 @@
         <v>68</v>
       </c>
       <c r="D2" s="50" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E2" s="77">
         <v>1</v>
@@ -4046,10 +4049,10 @@
         <v>12</v>
       </c>
       <c r="G2" s="51" t="s">
+        <v>87</v>
+      </c>
+      <c r="H2" s="50" t="s">
         <v>88</v>
-      </c>
-      <c r="H2" s="50" t="s">
-        <v>89</v>
       </c>
       <c r="I2" s="70" t="s">
         <v>67</v>
@@ -4063,7 +4066,7 @@
         <v>57</v>
       </c>
       <c r="D3" s="54" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E3" s="78">
         <v>1</v>
@@ -4072,10 +4075,10 @@
         <v>13</v>
       </c>
       <c r="G3" s="55" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H3" s="71" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I3" s="72" t="s">
         <v>58</v>
@@ -4089,7 +4092,7 @@
         <v>56</v>
       </c>
       <c r="D4" s="53" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E4" s="79">
         <v>1</v>
@@ -4098,10 +4101,10 @@
         <v>13</v>
       </c>
       <c r="G4" s="53" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H4" s="54" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I4" s="73" t="s">
         <v>60</v>
@@ -4115,7 +4118,7 @@
         <v>20</v>
       </c>
       <c r="D5" s="54" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E5" s="79">
         <v>0</v>
@@ -4124,7 +4127,7 @@
         <v>13</v>
       </c>
       <c r="G5" s="76" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H5" s="54" t="s">
         <v>50</v>
@@ -4141,7 +4144,7 @@
         <v>26</v>
       </c>
       <c r="D6" s="50" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E6" s="77">
         <v>3</v>
@@ -4167,7 +4170,7 @@
         <v>27</v>
       </c>
       <c r="D7" s="53" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E7" s="78">
         <v>2</v>
@@ -4176,7 +4179,7 @@
         <v>12</v>
       </c>
       <c r="G7" s="55" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H7" s="53" t="s">
         <v>66</v>
@@ -4193,7 +4196,7 @@
         <v>16</v>
       </c>
       <c r="D8" s="53" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E8" s="78">
         <v>2</v>
@@ -4219,7 +4222,7 @@
         <v>18</v>
       </c>
       <c r="D9" s="57" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E9" s="80">
         <v>2</v>
@@ -4234,7 +4237,7 @@
         <v>63</v>
       </c>
       <c r="I9" s="74" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="17" x14ac:dyDescent="0.2">
@@ -4244,7 +4247,7 @@
     </row>
     <row r="15" spans="2:9" ht="85" x14ac:dyDescent="0.2">
       <c r="C15" s="32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -4271,12 +4274,12 @@
         <v>2</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="40" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B2" s="41" t="s">
         <v>52</v>
@@ -4284,10 +4287,10 @@
     </row>
     <row r="3" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="40" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B3" s="42" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4300,7 +4303,7 @@
     </row>
     <row r="5" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="40" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B5" s="41" t="s">
         <v>54</v>
@@ -4308,7 +4311,7 @@
     </row>
     <row r="6" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="43" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B6" s="44" t="s">
         <v>55</v>
@@ -4339,7 +4342,7 @@
     <row r="12" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="35"/>
       <c r="B12" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -4360,44 +4363,46 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1D8EA89-DADA-994F-B9EB-DFFAA747018D}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="2" max="2" width="24.83203125" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="1" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="24.83203125" customWidth="1"/>
     <col min="4" max="4" width="27.33203125" customWidth="1"/>
-    <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="24.6640625" customWidth="1"/>
-    <col min="7" max="7" width="20" customWidth="1"/>
+    <col min="5" max="5" width="11.5" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" t="s">
         <v>120</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>121</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H1" t="s">
         <v>71</v>
-      </c>
-      <c r="D1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F1" t="s">
-        <v>124</v>
-      </c>
-      <c r="G1" t="s">
-        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adjusted starting values - improved estimates
fixed sigmas
</commit_message>
<xml_diff>
--- a/writing/Manuscript_Tables.xlsx
+++ b/writing/Manuscript_Tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/genoasullaway/Documents/GitHub/AYK_prey/writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417E0854-9018-884D-A50F-129AFBDDEC9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED4CBF1-AFDC-EF4E-A25F-21D78E804951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3940" yWindow="760" windowWidth="30620" windowHeight="20340" activeTab="3" xr2:uid="{15635B22-154F-5C4D-8D09-E55D0FC35932}"/>
+    <workbookView xWindow="160" yWindow="920" windowWidth="34240" windowHeight="21260" activeTab="1" xr2:uid="{15635B22-154F-5C4D-8D09-E55D0FC35932}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1 Priors" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="132">
   <si>
     <t>Stage</t>
   </si>
@@ -458,6 +458,21 @@
   </si>
   <si>
     <t>Parameter Notation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insulating properties of snow </t>
+  </si>
+  <si>
+    <t>Alaska Climate Research Center</t>
+  </si>
+  <si>
+    <t>Raymond-Yakoubian J 2009, Jallen et al 2022</t>
+  </si>
+  <si>
+    <t>Monthly Mean Snow Depth (in), summed October - December, 2002-2022</t>
+  </si>
+  <si>
+    <t>Snow Depth</t>
   </si>
 </sst>
 </file>
@@ -540,7 +555,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -979,12 +994,47 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1184,9 +1234,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1196,9 +1243,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1233,6 +1277,39 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3501,8 +3578,8 @@
       <xdr:rowOff>201448</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="386516" cy="173766"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -3587,7 +3664,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -3660,8 +3737,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="450829" cy="173766"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -3746,7 +3823,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -3819,8 +3896,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="499945" cy="173766"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3">
@@ -3905,7 +3982,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3">
@@ -3978,8 +4055,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="520079" cy="182871"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -4064,7 +4141,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -4137,8 +4214,8 @@
       <xdr:rowOff>11385</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="100156" cy="173766"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6">
@@ -4202,7 +4279,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6">
@@ -4268,8 +4345,8 @@
       <xdr:rowOff>2628</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="141256" cy="173766"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
@@ -4354,7 +4431,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
@@ -4427,8 +4504,8 @@
       <xdr:rowOff>7007</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="160621" cy="173702"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8">
@@ -4513,7 +4590,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8">
@@ -4586,8 +4663,8 @@
       <xdr:rowOff>28904</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="172035" cy="173702"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9">
@@ -4670,7 +4747,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9">
@@ -4742,8 +4819,8 @@
       <xdr:rowOff>2626</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="106632" cy="173702"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="TextBox 10">
@@ -4806,7 +4883,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="TextBox 10">
@@ -4871,8 +4948,8 @@
       <xdr:rowOff>8829</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="182614" cy="173702"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="TextBox 11">
@@ -4955,7 +5032,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="TextBox 11">
@@ -5027,8 +5104,8 @@
       <xdr:rowOff>17224</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="128112" cy="173702"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="13" name="TextBox 12">
@@ -5091,7 +5168,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="13" name="TextBox 12">
@@ -5156,8 +5233,8 @@
       <xdr:rowOff>215900</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="246414" cy="176651"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="14" name="TextBox 13">
@@ -5305,7 +5382,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="14" name="TextBox 13">
@@ -5899,10 +5976,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C922C39-C49D-8D4D-BCBE-7247337ED328}">
-  <dimension ref="B1:I15"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5919,7 +5996,7 @@
     <col min="11" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="46" t="s">
         <v>92</v>
       </c>
@@ -5945,221 +6022,251 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="2:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="B2" s="49" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="50" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" s="50" t="s">
-        <v>112</v>
+    <row r="2" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="B2" s="95" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="54" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="54" t="s">
+        <v>115</v>
       </c>
       <c r="E2" s="77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" s="81" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="51" t="s">
-        <v>87</v>
-      </c>
-      <c r="H2" s="50" t="s">
-        <v>88</v>
-      </c>
-      <c r="I2" s="70" t="s">
-        <v>67</v>
+        <v>13</v>
+      </c>
+      <c r="G2" s="74" t="s">
+        <v>89</v>
+      </c>
+      <c r="H2" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" s="71" t="s">
+        <v>69</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="102" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A3" s="18"/>
       <c r="B3" s="52" t="s">
         <v>30</v>
       </c>
       <c r="C3" s="53" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3" s="53" t="s">
+        <v>130</v>
+      </c>
+      <c r="E3" s="76">
+        <v>0</v>
+      </c>
+      <c r="F3" s="80" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="93" t="s">
+        <v>127</v>
+      </c>
+      <c r="H3" s="53" t="s">
+        <v>129</v>
+      </c>
+      <c r="I3" s="72" t="s">
+        <v>128</v>
+      </c>
+      <c r="J3" s="94"/>
+    </row>
+    <row r="4" spans="1:10" s="10" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A4" s="18"/>
+      <c r="B4" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="53" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" s="76">
+        <v>1</v>
+      </c>
+      <c r="F4" s="80" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="55" t="s">
+        <v>87</v>
+      </c>
+      <c r="H4" s="53" t="s">
+        <v>88</v>
+      </c>
+      <c r="I4" s="72" t="s">
+        <v>67</v>
+      </c>
+      <c r="J4" s="94"/>
+    </row>
+    <row r="5" spans="1:10" ht="102" x14ac:dyDescent="0.2">
+      <c r="B5" s="88" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="89" t="s">
         <v>57</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D5" s="86" t="s">
         <v>113</v>
       </c>
-      <c r="E3" s="78">
+      <c r="E5" s="90">
         <v>1</v>
       </c>
-      <c r="F3" s="82" t="s">
+      <c r="F5" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="55" t="s">
+      <c r="G5" s="92" t="s">
         <v>91</v>
       </c>
-      <c r="H3" s="71" t="s">
+      <c r="H5" s="96" t="s">
         <v>102</v>
       </c>
-      <c r="I3" s="72" t="s">
+      <c r="I5" s="87" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="B4" s="52" t="s">
+    <row r="6" spans="1:10" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C6" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="D4" s="53" t="s">
+      <c r="D6" s="53" t="s">
         <v>114</v>
       </c>
-      <c r="E4" s="79">
+      <c r="E6" s="77">
         <v>1</v>
       </c>
-      <c r="F4" s="83" t="s">
+      <c r="F6" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="53" t="s">
+      <c r="G6" s="53" t="s">
         <v>101</v>
       </c>
-      <c r="H4" s="54" t="s">
+      <c r="H6" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="I4" s="73" t="s">
+      <c r="I6" s="72" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="75" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="54" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="54" t="s">
-        <v>115</v>
-      </c>
-      <c r="E5" s="79">
-        <v>0</v>
-      </c>
-      <c r="F5" s="83" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="76" t="s">
-        <v>89</v>
-      </c>
-      <c r="H5" s="54" t="s">
-        <v>50</v>
-      </c>
-      <c r="I5" s="72" t="s">
-        <v>69</v>
+    <row r="7" spans="1:10" ht="102" x14ac:dyDescent="0.2">
+      <c r="B7" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="50" t="s">
+        <v>116</v>
+      </c>
+      <c r="E7" s="75">
+        <v>3</v>
+      </c>
+      <c r="F7" s="79" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="51" t="s">
+        <v>65</v>
+      </c>
+      <c r="H7" s="50" t="s">
+        <v>66</v>
+      </c>
+      <c r="I7" s="70" t="s">
+        <v>59</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="B6" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="50" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="50" t="s">
-        <v>116</v>
-      </c>
-      <c r="E6" s="77">
-        <v>3</v>
-      </c>
-      <c r="F6" s="81" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="51" t="s">
-        <v>65</v>
-      </c>
-      <c r="H6" s="50" t="s">
-        <v>66</v>
-      </c>
-      <c r="I6" s="70" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="B7" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="53" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="53" t="s">
-        <v>116</v>
-      </c>
-      <c r="E7" s="78">
-        <v>2</v>
-      </c>
-      <c r="F7" s="82" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="55" t="s">
-        <v>100</v>
-      </c>
-      <c r="H7" s="53" t="s">
-        <v>66</v>
-      </c>
-      <c r="I7" s="73" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" ht="153" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="102" x14ac:dyDescent="0.2">
       <c r="B8" s="52" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="53" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="53" t="s">
+        <v>116</v>
+      </c>
+      <c r="E8" s="76">
+        <v>2</v>
+      </c>
+      <c r="F8" s="80" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="55" t="s">
+        <v>100</v>
+      </c>
+      <c r="H8" s="53" t="s">
+        <v>66</v>
+      </c>
+      <c r="I8" s="72" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="153" x14ac:dyDescent="0.2">
+      <c r="B9" s="52" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="53" t="s">
+      <c r="D9" s="53" t="s">
         <v>117</v>
       </c>
-      <c r="E8" s="78">
+      <c r="E9" s="76">
         <v>2</v>
       </c>
-      <c r="F8" s="82" t="s">
+      <c r="F9" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="53" t="s">
+      <c r="G9" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="H8" s="53" t="s">
+      <c r="H9" s="53" t="s">
         <v>63</v>
       </c>
-      <c r="I8" s="73" t="s">
+      <c r="I9" s="72" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="103" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="56" t="s">
+    <row r="10" spans="1:10" ht="103" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="57" t="s">
+      <c r="C10" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="57" t="s">
+      <c r="D10" s="57" t="s">
         <v>118</v>
       </c>
-      <c r="E9" s="80">
+      <c r="E10" s="78">
         <v>2</v>
       </c>
-      <c r="F9" s="84" t="s">
+      <c r="F10" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="57" t="s">
+      <c r="G10" s="57" t="s">
         <v>64</v>
       </c>
-      <c r="H9" s="57" t="s">
+      <c r="H10" s="57" t="s">
         <v>63</v>
       </c>
-      <c r="I9" s="74" t="s">
+      <c r="I10" s="73" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="2:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="C14" s="33" t="s">
+    <row r="15" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="C15" s="33" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="2:9" ht="85" x14ac:dyDescent="0.2">
-      <c r="C15" s="32" t="s">
+    <row r="16" spans="1:10" ht="85" x14ac:dyDescent="0.2">
+      <c r="C16" s="32" t="s">
         <v>104</v>
       </c>
     </row>
@@ -6278,7 +6385,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1D8EA89-DADA-994F-B9EB-DFFAA747018D}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
+    <sheetView zoomScale="93" workbookViewId="0">
       <selection activeCell="G2" sqref="G2:G13"/>
     </sheetView>
   </sheetViews>
@@ -6466,11 +6573,11 @@
       <c r="F1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="85" t="s">
+      <c r="G1" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="86"/>
-      <c r="I1" s="87"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="85"/>
     </row>
     <row r="2" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B2" s="7" t="s">

</xml_diff>

<commit_message>
updated estimate - trying to figure out best sigmas
</commit_message>
<xml_diff>
--- a/writing/Manuscript_Tables.xlsx
+++ b/writing/Manuscript_Tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/genoasullaway/Documents/GitHub/AYK_prey/writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED4CBF1-AFDC-EF4E-A25F-21D78E804951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AF780B7-5BF0-4142-845B-03DBF6080234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="920" windowWidth="34240" windowHeight="21260" activeTab="1" xr2:uid="{15635B22-154F-5C4D-8D09-E55D0FC35932}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="131">
   <si>
     <t>Stage</t>
   </si>
@@ -445,12 +445,6 @@
     <t>95% CI</t>
   </si>
   <si>
-    <t>R Hat</t>
-  </si>
-  <si>
-    <t>Effective Sample Size</t>
-  </si>
-  <si>
     <t>currently fixed:</t>
   </si>
   <si>
@@ -473,6 +467,9 @@
   </si>
   <si>
     <t>Snow Depth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table S2: Parameter definitions, priors and parameter estimates with 95% credible intervals.  </t>
   </si>
 </sst>
 </file>
@@ -1034,7 +1031,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1183,9 +1180,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1270,6 +1264,39 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1279,38 +1306,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5817,154 +5817,154 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="64" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="59" t="s">
+      <c r="C1" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="65" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="2" spans="2:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="B2" s="67"/>
-      <c r="C2" s="60" t="s">
+      <c r="B2" s="66"/>
+      <c r="C2" s="59" t="s">
         <v>73</v>
       </c>
-      <c r="D2" s="68" t="s">
+      <c r="D2" s="67" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B3" s="67"/>
-      <c r="C3" s="60" t="s">
+      <c r="B3" s="66"/>
+      <c r="C3" s="59" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="68" t="s">
+      <c r="D3" s="67" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B4" s="67"/>
-      <c r="C4" s="60" t="s">
+      <c r="B4" s="66"/>
+      <c r="C4" s="59" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="68" t="s">
+      <c r="D4" s="67" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B5" s="67"/>
-      <c r="C5" s="60" t="s">
+      <c r="B5" s="66"/>
+      <c r="C5" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="D5" s="68" t="s">
+      <c r="D5" s="67" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B6" s="67"/>
-      <c r="C6" s="60" t="s">
+      <c r="B6" s="66"/>
+      <c r="C6" s="59" t="s">
         <v>79</v>
       </c>
-      <c r="D6" s="68" t="s">
+      <c r="D6" s="67" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B7" s="67"/>
-      <c r="C7" s="60" t="s">
+      <c r="B7" s="66"/>
+      <c r="C7" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="D7" s="68" t="s">
+      <c r="D7" s="67" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B8" s="67"/>
-      <c r="C8" s="60" t="s">
-        <v>125</v>
-      </c>
-      <c r="D8" s="68" t="s">
+      <c r="B8" s="66"/>
+      <c r="C8" s="59" t="s">
+        <v>123</v>
+      </c>
+      <c r="D8" s="67" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B9" s="67"/>
-      <c r="C9" s="61" t="s">
+      <c r="B9" s="66"/>
+      <c r="C9" s="60" t="s">
         <v>84</v>
       </c>
-      <c r="D9" s="68" t="s">
+      <c r="D9" s="67" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="B10" s="67"/>
-      <c r="C10" s="61" t="s">
+      <c r="B10" s="66"/>
+      <c r="C10" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="D10" s="68" t="s">
+      <c r="D10" s="67" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="B11" s="67"/>
-      <c r="C11" s="61" t="s">
+      <c r="B11" s="66"/>
+      <c r="C11" s="60" t="s">
         <v>108</v>
       </c>
-      <c r="D11" s="68" t="s">
+      <c r="D11" s="67" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B12" s="67"/>
-      <c r="C12" s="58" t="s">
+      <c r="B12" s="66"/>
+      <c r="C12" s="57" t="s">
         <v>109</v>
       </c>
-      <c r="D12" s="68" t="s">
+      <c r="D12" s="67" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="69"/>
-      <c r="C13" s="62" t="s">
+      <c r="B13" s="68"/>
+      <c r="C13" s="61" t="s">
         <v>107</v>
       </c>
-      <c r="D13" s="68" t="s">
+      <c r="D13" s="67" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="C16" s="63" t="s">
+      <c r="C16" s="62" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="C17" s="64" t="s">
+      <c r="C17" s="63" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" s="45" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B23" s="67"/>
-      <c r="C23" s="60" t="s">
+      <c r="B23" s="66"/>
+      <c r="C23" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="D23" s="68" t="s">
+      <c r="D23" s="67" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B24" s="67"/>
-      <c r="C24" s="60" t="s">
+      <c r="B24" s="66"/>
+      <c r="C24" s="59" t="s">
         <v>82</v>
       </c>
-      <c r="D24" s="68" t="s">
+      <c r="D24" s="67" t="s">
         <v>106</v>
       </c>
     </row>
@@ -5978,8 +5978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C922C39-C49D-8D4D-BCBE-7247337ED328}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6023,136 +6023,136 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="B2" s="95" t="s">
+      <c r="B2" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="54" t="s">
+      <c r="D2" s="53" t="s">
         <v>115</v>
       </c>
-      <c r="E2" s="77">
+      <c r="E2" s="76">
         <v>0</v>
       </c>
-      <c r="F2" s="81" t="s">
+      <c r="F2" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="74" t="s">
+      <c r="G2" s="73" t="s">
         <v>89</v>
       </c>
-      <c r="H2" s="54" t="s">
+      <c r="H2" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="I2" s="71" t="s">
+      <c r="I2" s="70" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="18"/>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="53" t="s">
-        <v>131</v>
-      </c>
-      <c r="D3" s="53" t="s">
-        <v>130</v>
-      </c>
-      <c r="E3" s="76">
+      <c r="C3" s="52" t="s">
+        <v>129</v>
+      </c>
+      <c r="D3" s="52" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3" s="75">
         <v>0</v>
       </c>
-      <c r="F3" s="80" t="s">
+      <c r="F3" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="93" t="s">
+      <c r="G3" s="89" t="s">
+        <v>125</v>
+      </c>
+      <c r="H3" s="52" t="s">
         <v>127</v>
       </c>
-      <c r="H3" s="53" t="s">
-        <v>129</v>
-      </c>
-      <c r="I3" s="72" t="s">
-        <v>128</v>
-      </c>
-      <c r="J3" s="94"/>
+      <c r="I3" s="71" t="s">
+        <v>126</v>
+      </c>
+      <c r="J3" s="90"/>
     </row>
     <row r="4" spans="1:10" s="10" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A4" s="18"/>
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="53" t="s">
+      <c r="C4" s="52" t="s">
         <v>68</v>
       </c>
-      <c r="D4" s="53" t="s">
+      <c r="D4" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="E4" s="76">
+      <c r="E4" s="75">
         <v>1</v>
       </c>
-      <c r="F4" s="80" t="s">
+      <c r="F4" s="79" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="55" t="s">
+      <c r="G4" s="54" t="s">
         <v>87</v>
       </c>
-      <c r="H4" s="53" t="s">
+      <c r="H4" s="52" t="s">
         <v>88</v>
       </c>
-      <c r="I4" s="72" t="s">
+      <c r="I4" s="71" t="s">
         <v>67</v>
       </c>
-      <c r="J4" s="94"/>
+      <c r="J4" s="90"/>
     </row>
     <row r="5" spans="1:10" ht="102" x14ac:dyDescent="0.2">
-      <c r="B5" s="88" t="s">
+      <c r="B5" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="89" t="s">
+      <c r="C5" s="85" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="86" t="s">
+      <c r="D5" s="82" t="s">
         <v>113</v>
       </c>
-      <c r="E5" s="90">
+      <c r="E5" s="86">
         <v>1</v>
       </c>
-      <c r="F5" s="91" t="s">
+      <c r="F5" s="87" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="92" t="s">
+      <c r="G5" s="88" t="s">
         <v>91</v>
       </c>
-      <c r="H5" s="96" t="s">
+      <c r="H5" s="92" t="s">
         <v>102</v>
       </c>
-      <c r="I5" s="87" t="s">
+      <c r="I5" s="83" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="96" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="54" t="s">
+      <c r="C6" s="53" t="s">
         <v>56</v>
       </c>
       <c r="D6" s="53" t="s">
         <v>114</v>
       </c>
-      <c r="E6" s="77">
+      <c r="E6" s="76">
         <v>1</v>
       </c>
-      <c r="F6" s="81" t="s">
+      <c r="F6" s="80" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="53" t="s">
         <v>101</v>
       </c>
-      <c r="H6" s="54" t="s">
+      <c r="H6" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="I6" s="72" t="s">
+      <c r="I6" s="70" t="s">
         <v>60</v>
       </c>
     </row>
@@ -6161,103 +6161,103 @@
         <v>15</v>
       </c>
       <c r="C7" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="50" t="s">
+        <v>118</v>
+      </c>
+      <c r="E7" s="74">
+        <v>2</v>
+      </c>
+      <c r="F7" s="78" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="50" t="s">
+        <v>64</v>
+      </c>
+      <c r="H7" s="50" t="s">
+        <v>63</v>
+      </c>
+      <c r="I7" s="69" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="153" x14ac:dyDescent="0.2">
+      <c r="B8" s="51" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="52" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="52" t="s">
+        <v>117</v>
+      </c>
+      <c r="E8" s="75">
+        <v>2</v>
+      </c>
+      <c r="F8" s="79" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="52" t="s">
+        <v>62</v>
+      </c>
+      <c r="H8" s="52" t="s">
+        <v>63</v>
+      </c>
+      <c r="I8" s="71" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="102" x14ac:dyDescent="0.2">
+      <c r="B9" s="51" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="50" t="s">
+      <c r="D9" s="52" t="s">
         <v>116</v>
       </c>
-      <c r="E7" s="75">
+      <c r="E9" s="75">
         <v>3</v>
       </c>
-      <c r="F7" s="79" t="s">
+      <c r="F9" s="79" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="51" t="s">
+      <c r="G9" s="54" t="s">
         <v>65</v>
       </c>
-      <c r="H7" s="50" t="s">
+      <c r="H9" s="52" t="s">
         <v>66</v>
       </c>
-      <c r="I7" s="70" t="s">
+      <c r="I9" s="71" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="102" x14ac:dyDescent="0.2">
-      <c r="B8" s="52" t="s">
+    <row r="10" spans="1:10" ht="103" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="53" t="s">
+      <c r="C10" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="53" t="s">
+      <c r="D10" s="56" t="s">
         <v>116</v>
       </c>
-      <c r="E8" s="76">
+      <c r="E10" s="77">
         <v>2</v>
       </c>
-      <c r="F8" s="80" t="s">
+      <c r="F10" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="55" t="s">
+      <c r="G10" s="97" t="s">
         <v>100</v>
       </c>
-      <c r="H8" s="53" t="s">
+      <c r="H10" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="I8" s="72" t="s">
+      <c r="I10" s="72" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="153" x14ac:dyDescent="0.2">
-      <c r="B9" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="53" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="53" t="s">
-        <v>117</v>
-      </c>
-      <c r="E9" s="76">
-        <v>2</v>
-      </c>
-      <c r="F9" s="80" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="53" t="s">
-        <v>62</v>
-      </c>
-      <c r="H9" s="53" t="s">
-        <v>63</v>
-      </c>
-      <c r="I9" s="72" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="103" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="56" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="57" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="57" t="s">
-        <v>118</v>
-      </c>
-      <c r="E10" s="78">
-        <v>2</v>
-      </c>
-      <c r="F10" s="82" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="57" t="s">
-        <v>64</v>
-      </c>
-      <c r="H10" s="57" t="s">
-        <v>63</v>
-      </c>
-      <c r="I10" s="73" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -6280,7 +6280,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B11" sqref="B11:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6383,10 +6383,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1D8EA89-DADA-994F-B9EB-DFFAA747018D}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="93" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G13"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6395,14 +6395,12 @@
     <col min="2" max="2" width="24.83203125" customWidth="1"/>
     <col min="3" max="3" width="27.33203125" customWidth="1"/>
     <col min="4" max="4" width="11.5" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B1" t="s">
         <v>119</v>
@@ -6414,121 +6412,120 @@
         <v>121</v>
       </c>
       <c r="E1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A2" s="66"/>
+      <c r="B2" s="59" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" s="67" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="66"/>
+      <c r="B3" s="59" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" s="67" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="66"/>
+      <c r="B4" s="59" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="67" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="66"/>
+      <c r="B5" s="59" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" s="67" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="66"/>
+      <c r="B6" s="59" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" s="67" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="66"/>
+      <c r="B7" s="59" t="s">
+        <v>85</v>
+      </c>
+      <c r="E7" s="67" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="66"/>
+      <c r="B8" s="59" t="s">
         <v>123</v>
       </c>
-      <c r="F1" t="s">
-        <v>122</v>
-      </c>
-      <c r="G1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="67"/>
-      <c r="B2" s="60" t="s">
-        <v>73</v>
-      </c>
-      <c r="G2" s="68" t="s">
+      <c r="E8" s="67" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" s="67"/>
-      <c r="B3" s="60" t="s">
-        <v>74</v>
-      </c>
-      <c r="G3" s="68" t="s">
+    <row r="9" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A9" s="66"/>
+      <c r="B9" s="60" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" s="67" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="67"/>
-      <c r="B4" s="60" t="s">
-        <v>75</v>
-      </c>
-      <c r="G4" s="68" t="s">
+    <row r="10" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" s="66"/>
+      <c r="B10" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" s="67" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="67"/>
-      <c r="B5" s="60" t="s">
-        <v>76</v>
-      </c>
-      <c r="G5" s="68" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="67"/>
-      <c r="B6" s="60" t="s">
-        <v>79</v>
-      </c>
-      <c r="G6" s="68" t="s">
+    <row r="11" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A11" s="66"/>
+      <c r="B11" s="60" t="s">
+        <v>108</v>
+      </c>
+      <c r="E11" s="67" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="66"/>
+      <c r="B12" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E12" s="67" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="67"/>
-      <c r="B7" s="60" t="s">
-        <v>85</v>
-      </c>
-      <c r="G7" s="68" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="67"/>
-      <c r="B8" s="60" t="s">
-        <v>125</v>
-      </c>
-      <c r="G8" s="68" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A9" s="67"/>
-      <c r="B9" s="61" t="s">
-        <v>84</v>
-      </c>
-      <c r="G9" s="68" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10" s="67"/>
-      <c r="B10" s="61" t="s">
-        <v>83</v>
-      </c>
-      <c r="G10" s="68" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A11" s="67"/>
-      <c r="B11" s="61" t="s">
-        <v>108</v>
-      </c>
-      <c r="G11" s="68" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="67"/>
-      <c r="B12" s="58" t="s">
-        <v>109</v>
-      </c>
-      <c r="G12" s="68" t="s">
+    <row r="13" spans="1:5" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="68"/>
+      <c r="B13" s="61" t="s">
+        <v>107</v>
+      </c>
+      <c r="E13" s="67" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="69"/>
-      <c r="B13" s="62" t="s">
-        <v>107</v>
-      </c>
-      <c r="G13" s="68" t="s">
-        <v>78</v>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -6573,11 +6570,11 @@
       <c r="F1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="83" t="s">
+      <c r="G1" s="93" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="84"/>
-      <c r="I1" s="85"/>
+      <c r="H1" s="94"/>
+      <c r="I1" s="95"/>
     </row>
     <row r="2" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B2" s="7" t="s">

</xml_diff>

<commit_message>
a final run, for now!
using this run for estimates for curry first full draft
</commit_message>
<xml_diff>
--- a/writing/Manuscript_Tables.xlsx
+++ b/writing/Manuscript_Tables.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/genoasullaway/Documents/GitHub/AYK_prey/writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2853DC44-AE59-9643-91D8-17576E317F6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C49D5D-C599-A84F-8896-80EDAF6C4724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13380" yWindow="760" windowWidth="21000" windowHeight="21420" activeTab="4" xr2:uid="{15635B22-154F-5C4D-8D09-E55D0FC35932}"/>
   </bookViews>
   <sheets>
-    <sheet name="Table 1 Priors" sheetId="4" r:id="rId1"/>
-    <sheet name="Table 2 Covariates" sheetId="3" r:id="rId2"/>
+    <sheet name="Table 1 Covariates" sheetId="3" r:id="rId1"/>
+    <sheet name="Table 2 Priors" sheetId="4" r:id="rId2"/>
     <sheet name="Supplement Table 1" sheetId="5" r:id="rId3"/>
     <sheet name="Supplement Table 2 " sheetId="6" r:id="rId4"/>
     <sheet name="Supplement Table 3" sheetId="7" r:id="rId5"/>
@@ -1135,7 +1135,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1407,24 +1407,32 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5989,181 +5997,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F6D1E8C-B800-DB41-95B4-3695A974BBA7}">
-  <dimension ref="B1:D24"/>
-  <sheetViews>
-    <sheetView zoomScale="173" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.83203125" style="45"/>
-    <col min="2" max="2" width="15.83203125" style="45" customWidth="1"/>
-    <col min="3" max="3" width="47.6640625" style="45" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" style="45" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="45"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B1" s="64" t="s">
-        <v>69</v>
-      </c>
-      <c r="C1" s="58" t="s">
-        <v>71</v>
-      </c>
-      <c r="D1" s="65" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="2:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="B2" s="66"/>
-      <c r="C2" s="59" t="s">
-        <v>72</v>
-      </c>
-      <c r="D2" s="67" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B3" s="66"/>
-      <c r="C3" s="59" t="s">
-        <v>73</v>
-      </c>
-      <c r="D3" s="67" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B4" s="66"/>
-      <c r="C4" s="59" t="s">
-        <v>74</v>
-      </c>
-      <c r="D4" s="67" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B5" s="66"/>
-      <c r="C5" s="59" t="s">
-        <v>75</v>
-      </c>
-      <c r="D5" s="67" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B6" s="66"/>
-      <c r="C6" s="59" t="s">
-        <v>78</v>
-      </c>
-      <c r="D6" s="67" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B7" s="66"/>
-      <c r="C7" s="59" t="s">
-        <v>84</v>
-      </c>
-      <c r="D7" s="67" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B8" s="66"/>
-      <c r="C8" s="59" t="s">
-        <v>122</v>
-      </c>
-      <c r="D8" s="67" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B9" s="66"/>
-      <c r="C9" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="D9" s="67" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="B10" s="66"/>
-      <c r="C10" s="60" t="s">
-        <v>82</v>
-      </c>
-      <c r="D10" s="67" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="B11" s="66"/>
-      <c r="C11" s="60" t="s">
-        <v>107</v>
-      </c>
-      <c r="D11" s="67" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B12" s="66"/>
-      <c r="C12" s="57" t="s">
-        <v>108</v>
-      </c>
-      <c r="D12" s="67" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="68"/>
-      <c r="C13" s="61" t="s">
-        <v>106</v>
-      </c>
-      <c r="D13" s="67" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="C16" s="62" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="C17" s="63" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="45" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B23" s="66"/>
-      <c r="C23" s="59" t="s">
-        <v>80</v>
-      </c>
-      <c r="D23" s="67" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B24" s="66"/>
-      <c r="C24" s="59" t="s">
-        <v>81</v>
-      </c>
-      <c r="D24" s="67" t="s">
-        <v>105</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C922C39-C49D-8D4D-BCBE-7247337ED328}">
   <dimension ref="A1:J16"/>
   <sheetViews>
@@ -6461,6 +6294,181 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F6D1E8C-B800-DB41-95B4-3695A974BBA7}">
+  <dimension ref="B1:D24"/>
+  <sheetViews>
+    <sheetView zoomScale="173" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="45"/>
+    <col min="2" max="2" width="15.83203125" style="45" customWidth="1"/>
+    <col min="3" max="3" width="47.6640625" style="45" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" style="45" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="45"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B1" s="64" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="58" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="65" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="B2" s="66"/>
+      <c r="C2" s="59" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="67" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B3" s="66"/>
+      <c r="C3" s="59" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="67" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B4" s="66"/>
+      <c r="C4" s="59" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="67" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B5" s="66"/>
+      <c r="C5" s="59" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="67" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B6" s="66"/>
+      <c r="C6" s="59" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="67" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B7" s="66"/>
+      <c r="C7" s="59" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="67" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B8" s="66"/>
+      <c r="C8" s="59" t="s">
+        <v>122</v>
+      </c>
+      <c r="D8" s="67" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B9" s="66"/>
+      <c r="C9" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" s="67" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="B10" s="66"/>
+      <c r="C10" s="60" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="67" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="B11" s="66"/>
+      <c r="C11" s="60" t="s">
+        <v>107</v>
+      </c>
+      <c r="D11" s="67" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B12" s="66"/>
+      <c r="C12" s="57" t="s">
+        <v>108</v>
+      </c>
+      <c r="D12" s="67" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="68"/>
+      <c r="C13" s="61" t="s">
+        <v>106</v>
+      </c>
+      <c r="D13" s="67" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="C16" s="62" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="C17" s="63" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B22" s="45" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B23" s="66"/>
+      <c r="C23" s="59" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" s="67" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B24" s="66"/>
+      <c r="C24" s="59" t="s">
+        <v>81</v>
+      </c>
+      <c r="D24" s="67" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6728,95 +6736,95 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="26.6640625" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" style="107" customWidth="1"/>
     <col min="4" max="4" width="31.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="95" t="s">
         <v>131</v>
       </c>
-      <c r="B1" s="99" t="s">
+      <c r="B1" s="96" t="s">
         <v>132</v>
       </c>
-      <c r="C1" s="99" t="s">
+      <c r="C1" s="106" t="s">
         <v>130</v>
       </c>
-      <c r="D1" s="100" t="s">
+      <c r="D1" s="97" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="101" t="s">
+      <c r="A2" s="98" t="s">
         <v>133</v>
       </c>
-      <c r="B2" s="102" t="s">
+      <c r="B2" t="s">
         <v>143</v>
       </c>
-      <c r="C2" s="102">
+      <c r="C2" s="107">
         <v>4.1100000000000003</v>
       </c>
-      <c r="D2" s="103" t="s">
+      <c r="D2" s="99" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="101"/>
-      <c r="B3" s="102" t="s">
+      <c r="A3" s="98"/>
+      <c r="B3" t="s">
         <v>138</v>
       </c>
-      <c r="C3" s="102">
+      <c r="C3" s="107">
         <v>4.12</v>
       </c>
-      <c r="D3" s="103" t="s">
+      <c r="D3" s="99" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="101" t="s">
+      <c r="A4" s="98" t="s">
         <v>136</v>
       </c>
-      <c r="B4" s="102" t="s">
+      <c r="B4" t="s">
         <v>142</v>
       </c>
-      <c r="C4" s="102">
+      <c r="C4" s="107">
         <v>4.13</v>
       </c>
-      <c r="D4" s="103" t="s">
+      <c r="D4" s="99" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="101" t="s">
+      <c r="A5" s="98" t="s">
         <v>141</v>
       </c>
-      <c r="B5" s="102" t="s">
+      <c r="B5" t="s">
         <v>140</v>
       </c>
-      <c r="C5" s="102">
+      <c r="C5" s="107">
         <v>4.1399999999999997</v>
       </c>
-      <c r="D5" s="103" t="s">
+      <c r="D5" s="99" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="104" t="s">
+      <c r="A6" s="100" t="s">
         <v>137</v>
       </c>
-      <c r="B6" s="105" t="s">
+      <c r="B6" s="101" t="s">
         <v>139</v>
       </c>
-      <c r="C6" s="105">
+      <c r="C6" s="108">
         <v>4.1500000000000004</v>
       </c>
-      <c r="D6" s="106" t="s">
+      <c r="D6" s="102" t="s">
         <v>135</v>
       </c>
     </row>
@@ -6872,11 +6880,11 @@
       <c r="F1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="95" t="s">
+      <c r="G1" s="103" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="96"/>
-      <c r="I1" s="97"/>
+      <c r="H1" s="104"/>
+      <c r="I1" s="105"/>
     </row>
     <row r="2" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B2" s="7" t="s">

</xml_diff>